<commit_message>
Début d'implémentation de l'authentification
</commit_message>
<xml_diff>
--- a/routes.xlsx
+++ b/routes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\Mon Drive\FORMATION 2022\P7\P7_OPENCLASSROOMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0CE0800-9246-450C-AE4F-CCFA6FEDA7E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49C776D8-184D-4D8C-9993-1B9DEC1DAD8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1370" yWindow="1770" windowWidth="36000" windowHeight="18720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -507,7 +507,7 @@
   <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E27"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Début de l'implémentation de l'affichage des posts
</commit_message>
<xml_diff>
--- a/routes.xlsx
+++ b/routes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\Mon Drive\FORMATION 2022\P7\P7_OPENCLASSROOMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49C776D8-184D-4D8C-9993-1B9DEC1DAD8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEECE1E7-4239-4B1C-B41C-8344C64D62B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1370" yWindow="1770" windowWidth="36000" windowHeight="18720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -507,7 +507,7 @@
   <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Suppression de post depuis le front end avec debut de gestion de l'utilisateur admis ou non à supprimer
</commit_message>
<xml_diff>
--- a/routes.xlsx
+++ b/routes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\Mon Drive\FORMATION 2022\P7\P7_OPENCLASSROOMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEECE1E7-4239-4B1C-B41C-8344C64D62B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0D5C0DF-FC4D-4C4C-B8D4-BED4A7748341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1370" yWindow="1770" windowWidth="36000" windowHeight="18720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -507,7 +507,7 @@
   <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Lecture des commentaires pour chaque post
</commit_message>
<xml_diff>
--- a/routes.xlsx
+++ b/routes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\Mon Drive\FORMATION 2022\P7\P7_OPENCLASSROOMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0D5C0DF-FC4D-4C4C-B8D4-BED4A7748341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7D1FA04-77B9-4B9F-8ED7-78DCE9AEEA96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1370" yWindow="1770" windowWidth="36000" windowHeight="18720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -507,7 +507,7 @@
   <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Debuggage côté requete sql non dynamique
</commit_message>
<xml_diff>
--- a/routes.xlsx
+++ b/routes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\Mon Drive\FORMATION 2022\P7\P7_OPENCLASSROOMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7D1FA04-77B9-4B9F-8ED7-78DCE9AEEA96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{052A60DF-D980-4789-8490-6953C5BF19C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1370" yWindow="1770" windowWidth="36000" windowHeight="18720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -507,7 +507,7 @@
   <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Liaison front et back pour la route ajout de like
</commit_message>
<xml_diff>
--- a/routes.xlsx
+++ b/routes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\Mon Drive\FORMATION 2022\P7\P7_OPENCLASSROOMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{052A60DF-D980-4789-8490-6953C5BF19C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60B88C73-05ED-494E-9D0D-2D342616AAA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1370" yWindow="1770" windowWidth="36000" windowHeight="18720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -507,7 +507,7 @@
   <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="A19" sqref="A19:E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>